<commit_message>
Test programs skeleton and spreadsheets
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_model_full.xlsx
+++ b/tests/databooks/databook_model_full.xlsx
@@ -11,16 +11,18 @@
     <sheet name="Population Contacts" sheetId="2" r:id="rId2"/>
     <sheet name="Transfer Definitions" sheetId="3" r:id="rId3"/>
     <sheet name="Transfer Details" sheetId="4" r:id="rId4"/>
-    <sheet name="General Demographics" sheetId="5" r:id="rId5"/>
-    <sheet name="Epidemic Characteristics" sheetId="6" r:id="rId6"/>
-    <sheet name="Prevalence" sheetId="7" r:id="rId7"/>
+    <sheet name="Program Definitions" sheetId="8" r:id="rId5"/>
+    <sheet name="Program Details" sheetId="9" r:id="rId6"/>
+    <sheet name="General Demographics" sheetId="5" r:id="rId7"/>
+    <sheet name="Epidemic Characteristics" sheetId="6" r:id="rId8"/>
+    <sheet name="Prevalence" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -153,12 +155,65 @@
   <si>
     <t>Release</t>
   </si>
+  <si>
+    <t>DS Treatment Program</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>Cost-Coverage Details</t>
+  </si>
+  <si>
+    <t>Program Coverage</t>
+  </si>
+  <si>
+    <t>Program Funding</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Impact Attributes</t>
+  </si>
+  <si>
+    <t>MDR Treatment Program</t>
+  </si>
+  <si>
+    <t>Susceptible Vaccination Program</t>
+  </si>
+  <si>
+    <t>Latent Cure Program</t>
+  </si>
+  <si>
+    <t>ds-tb</t>
+  </si>
+  <si>
+    <t>mdr-tb</t>
+  </si>
+  <si>
+    <t>vac-tb</t>
+  </si>
+  <si>
+    <t>cure-tb</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,13 +239,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,7 +552,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +640,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +744,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B14" sqref="B14:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,10 +2393,1192 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>'Population Definitions'!$B$2</f>
+        <v>0-14</v>
+      </c>
+      <c r="D1" t="str">
+        <f>'Population Definitions'!$B$3</f>
+        <v>15-49</v>
+      </c>
+      <c r="E1" t="str">
+        <f>'Population Definitions'!$B$4</f>
+        <v>50+</v>
+      </c>
+      <c r="F1" t="str">
+        <f>'Population Definitions'!$B$5</f>
+        <v>Pris</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:F5">
+      <formula1>"n,y"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>'Program Definitions'!$A$2</f>
+        <v>DS Treatment Program</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>2000</v>
+      </c>
+      <c r="G2">
+        <v>2001</v>
+      </c>
+      <c r="H2">
+        <v>2002</v>
+      </c>
+      <c r="I2">
+        <v>2003</v>
+      </c>
+      <c r="J2">
+        <v>2004</v>
+      </c>
+      <c r="K2">
+        <v>2005</v>
+      </c>
+      <c r="L2">
+        <v>2006</v>
+      </c>
+      <c r="M2">
+        <v>2007</v>
+      </c>
+      <c r="N2">
+        <v>2008</v>
+      </c>
+      <c r="O2">
+        <v>2009</v>
+      </c>
+      <c r="P2">
+        <v>2010</v>
+      </c>
+      <c r="Q2">
+        <v>2011</v>
+      </c>
+      <c r="R2">
+        <v>2012</v>
+      </c>
+      <c r="S2">
+        <v>2013</v>
+      </c>
+      <c r="T2">
+        <v>2014</v>
+      </c>
+      <c r="U2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="str">
+        <f>IF(SUMPRODUCT(--(F3:U3&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3">
+        <f>SUM('General Demographics'!C2:C4)*0.5</f>
+        <v>305000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="str">
+        <f>IF(SUMPRODUCT(--(F4:U4&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2">
+        <f>U3*100</f>
+        <v>30500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="str">
+        <f>CONCATENATE("Unit Cost Estimate",IF(C3="Fraction"," (Per 1%)",""))</f>
+        <v>Unit Cost Estimate</v>
+      </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE(C4)</f>
+        <v>USD</v>
+      </c>
+      <c r="D5">
+        <f>IF(SUMPRODUCT(--(F5:U5&lt;&gt;"..."))=0,U4/U3,"N.A.")</f>
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="str">
+        <f>IF(B1="Latent Cure Program","Efficacy of Vaccination",IF(B1="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B1="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B1="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <v>Efficacy of treatment (After Treatment Completion)</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(B6&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(B6&lt;&gt;"...",IF(SUMPRODUCT(--(F6:U6&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E6" t="str">
+        <f>IF(B6&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="str">
+        <f>IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Adherence Probability (Yearly)",IF(B1="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <v>Adherence Probability (Yearly)</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(B7&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(B7&lt;&gt;"...",IF(SUMPRODUCT(--(F7:U7&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E7" t="str">
+        <f>IF(B7&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="str">
+        <f>IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Treatment Duration (Months)",IF(B1="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <v>Treatment Duration (Months)</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IF(B8&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D8">
+        <f>IF(B8&lt;&gt;"...",IF(SUMPRODUCT(--(F8:U8&lt;&gt;""))=0,12,"N.A."),"")</f>
+        <v>12</v>
+      </c>
+      <c r="E8" t="str">
+        <f>IF(B8&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>'Program Definitions'!$A$3</f>
+        <v>MDR Treatment Program</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>2000</v>
+      </c>
+      <c r="G11">
+        <v>2001</v>
+      </c>
+      <c r="H11">
+        <v>2002</v>
+      </c>
+      <c r="I11">
+        <v>2003</v>
+      </c>
+      <c r="J11">
+        <v>2004</v>
+      </c>
+      <c r="K11">
+        <v>2005</v>
+      </c>
+      <c r="L11">
+        <v>2006</v>
+      </c>
+      <c r="M11">
+        <v>2007</v>
+      </c>
+      <c r="N11">
+        <v>2008</v>
+      </c>
+      <c r="O11">
+        <v>2009</v>
+      </c>
+      <c r="P11">
+        <v>2010</v>
+      </c>
+      <c r="Q11">
+        <v>2011</v>
+      </c>
+      <c r="R11">
+        <v>2012</v>
+      </c>
+      <c r="S11">
+        <v>2013</v>
+      </c>
+      <c r="T11">
+        <v>2014</v>
+      </c>
+      <c r="U11">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <f>IF(SUMPRODUCT(--(F12:U12&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13">
+        <f>IF(SUMPRODUCT(--(F13:U13&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="str">
+        <f>CONCATENATE("Unit Cost Estimate",IF(C12="Fraction"," (Per 1%)",""))</f>
+        <v>Unit Cost Estimate</v>
+      </c>
+      <c r="C14" t="str">
+        <f>CONCATENATE(C13)</f>
+        <v>USD</v>
+      </c>
+      <c r="D14">
+        <f>IF(SUMPRODUCT(--(F14:U14&lt;&gt;"..."))=0,200,"N.A.")</f>
+        <v>200</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" t="s">
+        <v>45</v>
+      </c>
+      <c r="O14" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>45</v>
+      </c>
+      <c r="R14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T14" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="str">
+        <f>IF(B10="Latent Cure Program","Efficacy of Vaccination",IF(B10="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B10="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B10="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <v>Efficacy of treatment (After Treatment Completion)</v>
+      </c>
+      <c r="C15" t="str">
+        <f>IF(B15&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D15">
+        <f>IF(B15&lt;&gt;"...",IF(SUMPRODUCT(--(F15:U15&lt;&gt;""))=0,1,"N.A."),"")</f>
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f>IF(B15&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="str">
+        <f>IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Adherence Probability (Yearly)",IF(B10="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <v>Adherence Probability (Yearly)</v>
+      </c>
+      <c r="C16" t="str">
+        <f>IF(B16&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D16">
+        <f>IF(B16&lt;&gt;"...",IF(SUMPRODUCT(--(F16:U16&lt;&gt;""))=0,0.2,"N.A."),"")</f>
+        <v>0.2</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(B16&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="str">
+        <f>IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Treatment Duration (Months)",IF(B10="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <v>Treatment Duration (Months)</v>
+      </c>
+      <c r="C17" t="str">
+        <f>IF(B17&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D17">
+        <f>IF(B17&lt;&gt;"...",IF(SUMPRODUCT(--(F17:U17&lt;&gt;""))=0,12,"N.A."),"")</f>
+        <v>12</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IF(B17&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>'Program Definitions'!$A$4</f>
+        <v>Susceptible Vaccination Program</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>2000</v>
+      </c>
+      <c r="G20">
+        <v>2001</v>
+      </c>
+      <c r="H20">
+        <v>2002</v>
+      </c>
+      <c r="I20">
+        <v>2003</v>
+      </c>
+      <c r="J20">
+        <v>2004</v>
+      </c>
+      <c r="K20">
+        <v>2005</v>
+      </c>
+      <c r="L20">
+        <v>2006</v>
+      </c>
+      <c r="M20">
+        <v>2007</v>
+      </c>
+      <c r="N20">
+        <v>2008</v>
+      </c>
+      <c r="O20">
+        <v>2009</v>
+      </c>
+      <c r="P20">
+        <v>2010</v>
+      </c>
+      <c r="Q20">
+        <v>2011</v>
+      </c>
+      <c r="R20">
+        <v>2012</v>
+      </c>
+      <c r="S20">
+        <v>2013</v>
+      </c>
+      <c r="T20">
+        <v>2014</v>
+      </c>
+      <c r="U20">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(SUMPRODUCT(--(F21:U21&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(SUMPRODUCT(--(F22:U22&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="2">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="str">
+        <f>CONCATENATE("Unit Cost Estimate",IF(C21="Fraction"," (Per 1%)",""))</f>
+        <v>Unit Cost Estimate</v>
+      </c>
+      <c r="C23" t="str">
+        <f>CONCATENATE(C22)</f>
+        <v>USD</v>
+      </c>
+      <c r="D23">
+        <f>IF(SUMPRODUCT(--(F23:U23&lt;&gt;"..."))=0,K22/K21,"N.A.")</f>
+        <v>500</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" t="s">
+        <v>45</v>
+      </c>
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" t="s">
+        <v>45</v>
+      </c>
+      <c r="P23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R23" t="s">
+        <v>45</v>
+      </c>
+      <c r="S23" t="s">
+        <v>45</v>
+      </c>
+      <c r="T23" t="s">
+        <v>45</v>
+      </c>
+      <c r="U23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="str">
+        <f>IF(B19="Latent Cure Program","Efficacy of Vaccination",IF(B19="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B19="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B19="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <v>Efficacy of Vaccination</v>
+      </c>
+      <c r="C24" t="str">
+        <f>IF(B24&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24" t="str">
+        <f>IF(B24&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="str">
+        <f>IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Adherence Probability (Yearly)",IF(B19="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <v>...</v>
+      </c>
+      <c r="C25" t="str">
+        <f>IF(B25&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(B25&lt;&gt;"...",IF(SUMPRODUCT(--(F25:U25&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <f>IF(B25&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="str">
+        <f>IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Treatment Duration (Months)",IF(B19="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <v>...</v>
+      </c>
+      <c r="C26" t="str">
+        <f>IF(B26&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <f>IF(B26&lt;&gt;"...",IF(SUMPRODUCT(--(F26:U26&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E26" t="str">
+        <f>IF(B26&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>'Program Definitions'!$A$5</f>
+        <v>Latent Cure Program</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>2000</v>
+      </c>
+      <c r="G29">
+        <v>2001</v>
+      </c>
+      <c r="H29">
+        <v>2002</v>
+      </c>
+      <c r="I29">
+        <v>2003</v>
+      </c>
+      <c r="J29">
+        <v>2004</v>
+      </c>
+      <c r="K29">
+        <v>2005</v>
+      </c>
+      <c r="L29">
+        <v>2006</v>
+      </c>
+      <c r="M29">
+        <v>2007</v>
+      </c>
+      <c r="N29">
+        <v>2008</v>
+      </c>
+      <c r="O29">
+        <v>2009</v>
+      </c>
+      <c r="P29">
+        <v>2010</v>
+      </c>
+      <c r="Q29">
+        <v>2011</v>
+      </c>
+      <c r="R29">
+        <v>2012</v>
+      </c>
+      <c r="S29">
+        <v>2013</v>
+      </c>
+      <c r="T29">
+        <v>2014</v>
+      </c>
+      <c r="U29">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="str">
+        <f>IF(SUMPRODUCT(--(F30:U30&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>0.5</v>
+      </c>
+      <c r="U30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="str">
+        <f>IF(SUMPRODUCT(--(F31:U31&lt;&gt;""))=0,0,"N.A.")</f>
+        <v>N.A.</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <f>P30/0.01*$D$32</f>
+        <v>50000</v>
+      </c>
+      <c r="U31" s="1">
+        <f>U30/0.01*$D$32</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="str">
+        <f>CONCATENATE("Unit Cost Estimate",IF(C30="Fraction"," (Per 1%)",""))</f>
+        <v>Unit Cost Estimate (Per 1%)</v>
+      </c>
+      <c r="C32" t="str">
+        <f>CONCATENATE(C31)</f>
+        <v>USD</v>
+      </c>
+      <c r="D32">
+        <f>IF(SUMPRODUCT(--(F32:U32&lt;&gt;"..."))=0,1000,"N.A.")</f>
+        <v>1000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" t="s">
+        <v>45</v>
+      </c>
+      <c r="I32" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" t="s">
+        <v>45</v>
+      </c>
+      <c r="K32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P32" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>45</v>
+      </c>
+      <c r="R32" t="s">
+        <v>45</v>
+      </c>
+      <c r="S32" t="s">
+        <v>45</v>
+      </c>
+      <c r="T32" t="s">
+        <v>45</v>
+      </c>
+      <c r="U32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="str">
+        <f>IF(B28="Latent Cure Program","Efficacy of Vaccination",IF(B28="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B28="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B28="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <v>Efficacy of Vaccination</v>
+      </c>
+      <c r="C33" t="str">
+        <f>IF(B33&lt;&gt;"...","Unique","")</f>
+        <v>Unique</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="str">
+        <f>IF(B33&lt;&gt;"...","OR","")</f>
+        <v>OR</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="str">
+        <f>IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Adherence Probability (Yearly)",IF(B28="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <v>...</v>
+      </c>
+      <c r="C34" t="str">
+        <f>IF(B34&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <f>IF(B34&lt;&gt;"...",IF(SUMPRODUCT(--(F34:U34&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <f>IF(B34&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="str">
+        <f>IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Treatment Duration (Months)",IF(B28="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <v>...</v>
+      </c>
+      <c r="C35" t="str">
+        <f>IF(B35&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <f>IF(B35&lt;&gt;"...",IF(SUMPRODUCT(--(F35:U35&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E35" t="str">
+        <f>IF(B35&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="9">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C33:C35 C24:C26 C15:C17 C6:C8">
+      <formula1>"Unique"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F32:U32 F23:U23 F14:U14 F5:U5">
+      <formula1>"..."</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C32">
+      <formula1>"=CONCATENATE(C31)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C31 C22 C13 C4">
+      <formula1>"USD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C30 C21 C12 C3">
+      <formula1>"Number,Fraction"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B28 B19 B10 B1">
+      <formula1>"DS Treatment Program,MDR Treatment Program,Susceptible Vaccination Program,Latent Cure Program"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C23">
+      <formula1>"=CONCATENATE(C22)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C14">
+      <formula1>"=CONCATENATE(C13)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"=CONCATENATE(C4)"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3028,13 +4269,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4198,12 +5437,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update databook with hypothetical program data
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_model_full.xlsx
+++ b/tests/databooks/databook_model_full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" tabRatio="974" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -202,9 +202,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -239,16 +242,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -555,9 +564,9 @@
       <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="5" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -643,9 +652,9 @@
       <selection activeCell="B2" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -747,9 +756,9 @@
       <selection activeCell="B14" sqref="B14:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.68359375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,14 +1163,14 @@
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.68359375" customWidth="1"/>
+    <col min="3" max="3" width="15.68359375" customWidth="1"/>
+    <col min="4" max="5" width="10.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Transfer Definitions'!A1</f>
         <v>Aging</v>
@@ -1221,7 +1230,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF('Transfer Definitions'!C2="y",'Population Definitions'!$A$2,"...")</f>
         <v>Children 0-14</v>
@@ -1247,7 +1256,7 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>IF('Transfer Definitions'!D2="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1273,7 +1282,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('Transfer Definitions'!E2="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1299,7 +1308,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('Transfer Definitions'!B3="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1325,7 +1334,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('Transfer Definitions'!D3="y",'Population Definitions'!$A$3,"...")</f>
         <v>Adults 15-49</v>
@@ -1351,7 +1360,7 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('Transfer Definitions'!E3="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1377,7 +1386,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('Transfer Definitions'!B4="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1403,7 +1412,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('Transfer Definitions'!C4="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1429,7 +1438,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('Transfer Definitions'!E4="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1455,7 +1464,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('Transfer Definitions'!B5="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1481,7 +1490,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('Transfer Definitions'!C5="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1507,7 +1516,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('Transfer Definitions'!D5="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1533,7 +1542,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'Transfer Definitions'!A7</f>
         <v>Incarceration</v>
@@ -1593,7 +1602,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('Transfer Definitions'!C8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1619,7 +1628,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('Transfer Definitions'!D8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1645,7 +1654,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('Transfer Definitions'!E8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1671,7 +1680,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('Transfer Definitions'!B9="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1697,7 +1706,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('Transfer Definitions'!D9="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1723,7 +1732,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('Transfer Definitions'!E9="y",'Population Definitions'!$A$3,"...")</f>
         <v>Adults 15-49</v>
@@ -1748,7 +1757,7 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('Transfer Definitions'!B10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1774,7 +1783,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('Transfer Definitions'!C10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1800,7 +1809,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('Transfer Definitions'!E10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1826,7 +1835,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('Transfer Definitions'!B11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1852,7 +1861,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('Transfer Definitions'!C11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1878,7 +1887,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('Transfer Definitions'!D11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1904,7 +1913,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>'Transfer Definitions'!A13</f>
         <v>Release</v>
@@ -1964,7 +1973,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('Transfer Definitions'!C14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1990,7 +1999,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('Transfer Definitions'!D14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -2016,7 +2025,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF('Transfer Definitions'!E14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -2042,7 +2051,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('Transfer Definitions'!B15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2068,7 +2077,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF('Transfer Definitions'!D15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2094,7 +2103,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF('Transfer Definitions'!E15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2120,7 +2129,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF('Transfer Definitions'!B16="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -2146,7 +2155,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF('Transfer Definitions'!C16="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -2172,7 +2181,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="str">
         <f>IF('Transfer Definitions'!E16="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -2198,7 +2207,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="str">
         <f>IF('Transfer Definitions'!B17="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -2224,7 +2233,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="str">
         <f>IF('Transfer Definitions'!C17="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -2250,7 +2259,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="str">
         <f>IF('Transfer Definitions'!D17="y",'Population Definitions'!$A$5,"...")</f>
         <v>Prisoners</v>
@@ -2399,14 +2408,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.68359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.68359375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2527,26 +2536,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.578125" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7890625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.15625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7890625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>'Program Definitions'!$A$2</f>
         <v>DS Treatment Program</v>
@@ -2555,7 +2568,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2614,7 +2627,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2631,12 +2644,17 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="U3">
-        <f>SUM('General Demographics'!C2:C4)*0.5</f>
-        <v>305000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="P3" s="4">
+        <f>U3/2</f>
+        <v>76250</v>
+      </c>
+      <c r="U3" s="3">
+        <f>SUM('General Demographics'!C2:C4)*0.25</f>
+        <v>152500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -2663,17 +2681,20 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
+      <c r="P4" s="2">
+        <f>P3*D5</f>
+        <v>7625000</v>
+      </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2">
-        <f>U3*100</f>
-        <v>30500000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <f>U3*D5</f>
+        <v>15250000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2686,7 +2707,7 @@
         <v>USD</v>
       </c>
       <c r="D5">
-        <f>IF(SUMPRODUCT(--(F5:U5&lt;&gt;"..."))=0,U4/U3,"N.A.")</f>
+        <f>IF(SUMPRODUCT(--(F5:U5&lt;&gt;"..."))=0,100,"N.A.")</f>
         <v>100</v>
       </c>
       <c r="E5" t="s">
@@ -2741,7 +2762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -2761,11 +2782,15 @@
         <f>IF(B6&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>0.75</v>
+      </c>
+      <c r="Q6" s="5"/>
+      <c r="U6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2785,11 +2810,15 @@
         <f>IF(B7&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P7" s="6">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="U7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2801,16 +2830,22 @@
         <f>IF(B8&lt;&gt;"...","Unique","")</f>
         <v>Unique</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="str">
         <f>IF(B8&lt;&gt;"...",IF(SUMPRODUCT(--(F8:U8&lt;&gt;""))=0,12,"N.A."),"")</f>
-        <v>12</v>
+        <v>N.A.</v>
       </c>
       <c r="E8" t="str">
         <f>IF(B8&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>12</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Program Definitions'!$A$3</f>
         <v>MDR Treatment Program</v>
@@ -2819,7 +2854,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2878,7 +2913,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -2888,15 +2923,19 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="str">
         <f>IF(SUMPRODUCT(--(F12:U12&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S12" s="3">
+        <f>SUM('General Demographics'!C3:C4)*0.05</f>
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2906,15 +2945,34 @@
       <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="str">
         <f>IF(SUMPRODUCT(--(F13:U13&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2">
+        <f>S12*D14</f>
+        <v>5100000</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2982,7 +3040,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2994,16 +3052,20 @@
         <f>IF(B15&lt;&gt;"...","Unique","")</f>
         <v>Unique</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="str">
         <f>IF(B15&lt;&gt;"...",IF(SUMPRODUCT(--(F15:U15&lt;&gt;""))=0,1,"N.A."),"")</f>
-        <v>1</v>
+        <v>N.A.</v>
       </c>
       <c r="E15" t="str">
         <f>IF(B15&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U15" s="6">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -3015,16 +3077,19 @@
         <f>IF(B16&lt;&gt;"...","Unique","")</f>
         <v>Unique</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="str">
         <f>IF(B16&lt;&gt;"...",IF(SUMPRODUCT(--(F16:U16&lt;&gt;""))=0,0.2,"N.A."),"")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="E16" t="str">
         <f>IF(B16&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -3037,15 +3102,15 @@
         <v>Unique</v>
       </c>
       <c r="D17">
-        <f>IF(B17&lt;&gt;"...",IF(SUMPRODUCT(--(F17:U17&lt;&gt;""))=0,12,"N.A."),"")</f>
-        <v>12</v>
+        <f>IF(B17&lt;&gt;"...",IF(SUMPRODUCT(--(F17:U17&lt;&gt;""))=0,18,"N.A."),"")</f>
+        <v>18</v>
       </c>
       <c r="E17" t="str">
         <f>IF(B17&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>'Program Definitions'!$A$4</f>
         <v>Susceptible Vaccination Program</v>
@@ -3054,7 +3119,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -3113,7 +3178,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -3121,7 +3186,7 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D21" t="str">
         <f>IF(SUMPRODUCT(--(F21:U21&lt;&gt;""))=0,0,"N.A.")</f>
@@ -3130,11 +3195,11 @@
       <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="K21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -3151,25 +3216,27 @@
       <c r="E22" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="2">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f>F21*'General Demographics'!C2*D23</f>
+        <v>10500</v>
+      </c>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
       <c r="B23" t="str">
         <f>CONCATENATE("Unit Cost Estimate",IF(C21="Fraction"," (Per 1%)",""))</f>
-        <v>Unit Cost Estimate</v>
+        <v>Unit Cost Estimate (Per 1%)</v>
       </c>
       <c r="C23" t="str">
         <f>CONCATENATE(C22)</f>
         <v>USD</v>
       </c>
       <c r="D23">
-        <f>IF(SUMPRODUCT(--(F23:U23&lt;&gt;"..."))=0,K22/K21,"N.A.")</f>
-        <v>500</v>
+        <f>IF(SUMPRODUCT(--(F23:U23&lt;&gt;"..."))=0,10.5,"N.A.")</f>
+        <v>10.5</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -3223,7 +3290,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -3236,6 +3303,7 @@
         <v>Unique</v>
       </c>
       <c r="D24">
+        <f>IF(B24&lt;&gt;"...",IF(SUMPRODUCT(--(F24:U24&lt;&gt;""))=0,0.5,"N.A."),"")</f>
         <v>0.5</v>
       </c>
       <c r="E24" t="str">
@@ -3243,7 +3311,7 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -3264,7 +3332,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3285,7 +3353,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
         <f>'Program Definitions'!$A$5</f>
         <v>Latent Cure Program</v>
@@ -3294,7 +3362,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -3353,7 +3421,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -3361,7 +3429,7 @@
         <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="str">
         <f>IF(SUMPRODUCT(--(F30:U30&lt;&gt;""))=0,0,"N.A.")</f>
@@ -3370,17 +3438,14 @@
       <c r="E30" t="s">
         <v>11</v>
       </c>
-      <c r="F30">
+      <c r="O30">
         <v>0</v>
-      </c>
-      <c r="P30">
-        <v>0.5</v>
       </c>
       <c r="U30">
         <v>0.9</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -3397,33 +3462,30 @@
       <c r="E31" t="s">
         <v>11</v>
       </c>
-      <c r="F31">
+      <c r="O31">
         <v>0</v>
       </c>
-      <c r="P31" s="1">
-        <f>P30/0.01*$D$32</f>
-        <v>50000</v>
-      </c>
+      <c r="P31" s="1"/>
       <c r="U31" s="1">
         <f>U30/0.01*$D$32</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>45</v>
       </c>
       <c r="B32" t="str">
         <f>CONCATENATE("Unit Cost Estimate",IF(C30="Fraction"," (Per 1%)",""))</f>
-        <v>Unit Cost Estimate (Per 1%)</v>
+        <v>Unit Cost Estimate</v>
       </c>
       <c r="C32" t="str">
         <f>CONCATENATE(C31)</f>
         <v>USD</v>
       </c>
       <c r="D32">
-        <f>IF(SUMPRODUCT(--(F32:U32&lt;&gt;"..."))=0,1000,"N.A.")</f>
-        <v>1000</v>
+        <f>IF(SUMPRODUCT(--(F32:U32&lt;&gt;"..."))=0,50,"N.A.")</f>
+        <v>50</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -3477,7 +3539,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -3490,14 +3552,15 @@
         <v>Unique</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <f>IF(B33&lt;&gt;"...",IF(SUMPRODUCT(--(F33:U33&lt;&gt;""))=0,0.2,"N.A."),"")</f>
+        <v>0.2</v>
       </c>
       <c r="E33" t="str">
         <f>IF(B33&lt;&gt;"...","OR","")</f>
         <v>OR</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -3518,7 +3581,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -3578,16 +3641,16 @@
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.68359375" customWidth="1"/>
+    <col min="2" max="3" width="10.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -3646,7 +3709,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3662,7 +3725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3678,7 +3741,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -3694,7 +3757,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -3710,7 +3773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3769,7 +3832,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3785,7 +3848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3801,7 +3864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -3817,7 +3880,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -3833,7 +3896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3892,7 +3955,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3908,7 +3971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3924,7 +3987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -3940,7 +4003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -3956,7 +4019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -4015,7 +4078,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4031,7 +4094,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4047,7 +4110,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4063,7 +4126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4079,7 +4142,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4138,7 +4201,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4154,7 +4217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4170,7 +4233,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4186,7 +4249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4275,13 +4338,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.68359375" customWidth="1"/>
+    <col min="2" max="3" width="10.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -4340,7 +4403,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4356,7 +4419,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4372,7 +4435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4388,7 +4451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4404,7 +4467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -4463,7 +4526,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4479,7 +4542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4495,7 +4558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4511,7 +4574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4527,7 +4590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4586,7 +4649,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4602,7 +4665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4618,7 +4681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4634,7 +4697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4650,7 +4713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4709,7 +4772,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4734,7 +4797,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4759,7 +4822,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4784,7 +4847,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4809,7 +4872,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -4868,7 +4931,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4884,7 +4947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4900,7 +4963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4916,7 +4979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4932,7 +4995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -4991,7 +5054,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5007,7 +5070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5023,7 +5086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5039,7 +5102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5055,7 +5118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -5114,7 +5177,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5130,7 +5193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5146,7 +5209,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5162,7 +5225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5178,7 +5241,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -5237,7 +5300,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5253,7 +5316,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5269,7 +5332,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5285,7 +5348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5301,7 +5364,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -5360,7 +5423,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5376,7 +5439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5392,7 +5455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5408,7 +5471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5445,13 +5508,13 @@
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.68359375" customWidth="1"/>
+    <col min="2" max="3" width="10.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -5510,7 +5573,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5526,7 +5589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5554,7 +5617,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5570,7 +5633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5586,7 +5649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -5645,7 +5708,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5661,7 +5724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5680,7 +5743,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5696,7 +5759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5712,7 +5775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5771,7 +5834,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5787,7 +5850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5806,7 +5869,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5822,7 +5885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5838,7 +5901,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -5897,7 +5960,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5913,7 +5976,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5932,7 +5995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5948,7 +6011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5964,7 +6027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -6023,7 +6086,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -6039,7 +6102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -6058,7 +6121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -6074,7 +6137,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -6090,7 +6153,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -6149,7 +6212,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -6165,7 +6228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -6184,7 +6247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -6200,7 +6263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>

</xml_diff>

<commit_message>
update databook with addition of fixed cost programs
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_model_full.xlsx
+++ b/tests/databooks/databook_model_full.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" tabRatio="974" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="18" windowWidth="16098" windowHeight="9660" tabRatio="974" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Cost-Coverage Details</t>
   </si>
   <si>
-    <t>Program Coverage</t>
-  </si>
-  <si>
     <t>Program Funding</t>
   </si>
   <si>
@@ -197,6 +194,12 @@
   <si>
     <t>cure-tb</t>
   </si>
+  <si>
+    <t>Fixed Cost Program</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
 </sst>
 </file>
 
@@ -206,8 +209,8 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -251,9 +254,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -583,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -597,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -611,7 +614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -625,7 +628,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -678,7 +681,7 @@
         <v>Pris</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>'Population Definitions'!$B$2</f>
         <v>0-14</v>
@@ -687,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'Population Definitions'!$B$3</f>
         <v>15-49</v>
@@ -705,7 +708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>50+</v>
@@ -722,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Pris</v>
@@ -782,7 +785,7 @@
         <v>Pris</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>'Population Definitions'!$B$2</f>
         <v>0-14</v>
@@ -797,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'Population Definitions'!$B$3</f>
         <v>15-49</v>
@@ -812,7 +815,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>50+</v>
@@ -827,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Pris</v>
@@ -842,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -863,7 +866,7 @@
         <v>Pris</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
         <f>'Population Definitions'!$B$2</f>
         <v>0-14</v>
@@ -878,7 +881,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
         <f>'Population Definitions'!$B$3</f>
         <v>15-49</v>
@@ -893,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>50+</v>
@@ -908,7 +911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Pris</v>
@@ -923,7 +926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -944,7 +947,7 @@
         <v>Pris</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
         <f>'Population Definitions'!$B$2</f>
         <v>0-14</v>
@@ -959,7 +962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
         <f>'Population Definitions'!$B$3</f>
         <v>15-49</v>
@@ -974,7 +977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
         <f>'Population Definitions'!$B$4</f>
         <v>50+</v>
@@ -989,7 +992,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
         <f>'Population Definitions'!$B$5</f>
         <v>Pris</v>
@@ -1542,7 +1545,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
         <f>'Transfer Definitions'!A7</f>
         <v>Incarceration</v>
@@ -1602,7 +1605,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
         <f>IF('Transfer Definitions'!C8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1628,7 +1631,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
         <f>IF('Transfer Definitions'!D8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1654,7 +1657,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="str">
         <f>IF('Transfer Definitions'!E8="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1680,7 +1683,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="str">
         <f>IF('Transfer Definitions'!B9="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1706,7 +1709,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
         <f>IF('Transfer Definitions'!D9="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -1732,7 +1735,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
         <f>IF('Transfer Definitions'!E9="y",'Population Definitions'!$A$3,"...")</f>
         <v>Adults 15-49</v>
@@ -1757,7 +1760,7 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
         <f>IF('Transfer Definitions'!B10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1783,7 +1786,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
         <f>IF('Transfer Definitions'!C10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1809,7 +1812,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="str">
         <f>IF('Transfer Definitions'!E10="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -1835,7 +1838,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="str">
         <f>IF('Transfer Definitions'!B11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1861,7 +1864,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="str">
         <f>IF('Transfer Definitions'!C11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1887,7 +1890,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="str">
         <f>IF('Transfer Definitions'!D11="y",'Population Definitions'!$A$5,"...")</f>
         <v>...</v>
@@ -1913,7 +1916,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="str">
         <f>'Transfer Definitions'!A13</f>
         <v>Release</v>
@@ -1973,7 +1976,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="str">
         <f>IF('Transfer Definitions'!C14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -1999,7 +2002,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="str">
         <f>IF('Transfer Definitions'!D14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -2025,7 +2028,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="str">
         <f>IF('Transfer Definitions'!E14="y",'Population Definitions'!$A$2,"...")</f>
         <v>...</v>
@@ -2051,7 +2054,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="str">
         <f>IF('Transfer Definitions'!B15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2077,7 +2080,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="str">
         <f>IF('Transfer Definitions'!D15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2103,7 +2106,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="str">
         <f>IF('Transfer Definitions'!E15="y",'Population Definitions'!$A$3,"...")</f>
         <v>...</v>
@@ -2129,7 +2132,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="str">
         <f>IF('Transfer Definitions'!B16="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -2155,7 +2158,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="str">
         <f>IF('Transfer Definitions'!C16="y",'Population Definitions'!$A$4,"...")</f>
         <v>...</v>
@@ -2402,10 +2405,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2442,12 +2445,12 @@
         <v>Pris</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -2462,12 +2465,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -2482,12 +2485,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
@@ -2502,12 +2505,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -2522,9 +2525,29 @@
         <v>39</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:F5">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:F6">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2534,10 +2557,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U35"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2559,7 +2582,7 @@
     <col min="21" max="21" width="12.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="str">
         <f>'Program Definitions'!$A$2</f>
         <v>DS Treatment Program</v>
@@ -2568,7 +2591,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2627,12 +2650,13 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>46</v>
       </c>
-      <c r="B3" t="s">
-        <v>47</v>
+      <c r="B3" t="str">
+        <f>IF(B1="Fixed Cost Program","...","Program Coverage")</f>
+        <v>Program Coverage</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -2654,15 +2678,15 @@
         <v>152500</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
       </c>
       <c r="D4" t="str">
         <f>IF(SUMPRODUCT(--(F4:U4&lt;&gt;""))=0,0,"N.A.")</f>
@@ -2694,12 +2718,12 @@
         <v>15250000</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="str">
-        <f>CONCATENATE("Unit Cost Estimate",IF(C3="Fraction"," (Per 1%)",""))</f>
+        <f>IF(B1="Fixed Cost Program","...",CONCATENATE("Unit Cost Estimate",IF(C3="Fraction"," (Per 1%)","")))</f>
         <v>Unit Cost Estimate</v>
       </c>
       <c r="C5" t="str">
@@ -2762,12 +2786,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(B1="Latent Cure Program","Efficacy of Vaccination",IF(B1="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B1="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B1="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <f>IF(B1="Fixed Cost Program","...",IF(B1="Latent Cure Program","Efficacy of Cure",IF(B1="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B1="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B1="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","...")))))</f>
         <v>Efficacy of treatment (After Treatment Completion)</v>
       </c>
       <c r="C6" t="str">
@@ -2790,12 +2814,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Adherence Probability (Yearly)",IF(B1="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <f>IF(B1="Fixed Cost Program","...",IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Adherence Probability (Yearly)",IF(B1="DS Treatment Program","Adherence Probability (Yearly)","...")))))</f>
         <v>Adherence Probability (Yearly)</v>
       </c>
       <c r="C7" t="str">
@@ -2818,12 +2842,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="str">
-        <f>IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Treatment Duration (Months)",IF(B1="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <f>IF(B1="Fixed Cost Program","...",IF(B1="Latent Cure Program","...",IF(B1="Susceptible Vaccination Program","...",IF(B1="MDR Treatment Program","Treatment Duration (Months)",IF(B1="DS Treatment Program","Treatment Duration (Months)","...")))))</f>
         <v>Treatment Duration (Months)</v>
       </c>
       <c r="C8" t="str">
@@ -2845,16 +2869,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
         <f>'Program Definitions'!$A$3</f>
         <v>MDR Treatment Program</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2913,12 +2937,13 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
-        <v>47</v>
+      <c r="B12" t="str">
+        <f>IF(B10="Fixed Cost Program","...","Program Coverage")</f>
+        <v>Program Coverage</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -2935,15 +2960,15 @@
         <v>25500</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>45</v>
       </c>
       <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
       </c>
       <c r="D13" t="str">
         <f>IF(SUMPRODUCT(--(F13:U13&lt;&gt;""))=0,0,"N.A.")</f>
@@ -2972,12 +2997,12 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>45</v>
       </c>
       <c r="B14" t="str">
-        <f>CONCATENATE("Unit Cost Estimate",IF(C12="Fraction"," (Per 1%)",""))</f>
+        <f>IF(B10="Fixed Cost Program","...",CONCATENATE("Unit Cost Estimate",IF(C12="Fraction"," (Per 1%)","")))</f>
         <v>Unit Cost Estimate</v>
       </c>
       <c r="C14" t="str">
@@ -3040,12 +3065,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(B10="Latent Cure Program","Efficacy of Vaccination",IF(B10="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B10="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B10="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <f>IF(B10="Fixed Cost Program","...",IF(B10="Latent Cure Program","Efficacy of Cure",IF(B10="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B10="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B10="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","...")))))</f>
         <v>Efficacy of treatment (After Treatment Completion)</v>
       </c>
       <c r="C15" t="str">
@@ -3065,12 +3090,12 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>45</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Adherence Probability (Yearly)",IF(B10="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <f>IF(B10="Fixed Cost Program","...",IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Adherence Probability (Yearly)",IF(B10="DS Treatment Program","Adherence Probability (Yearly)","...")))))</f>
         <v>Adherence Probability (Yearly)</v>
       </c>
       <c r="C16" t="str">
@@ -3089,12 +3114,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>45</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Treatment Duration (Months)",IF(B10="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <f>IF(B10="Fixed Cost Program","...",IF(B10="Latent Cure Program","...",IF(B10="Susceptible Vaccination Program","...",IF(B10="MDR Treatment Program","Treatment Duration (Months)",IF(B10="DS Treatment Program","Treatment Duration (Months)","...")))))</f>
         <v>Treatment Duration (Months)</v>
       </c>
       <c r="C17" t="str">
@@ -3110,16 +3135,16 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="str">
         <f>'Program Definitions'!$A$4</f>
         <v>Susceptible Vaccination Program</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -3178,12 +3203,13 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
-        <v>47</v>
+      <c r="B21" t="str">
+        <f>IF(B19="Fixed Cost Program","...","Program Coverage")</f>
+        <v>Program Coverage</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -3199,15 +3225,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>45</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
       </c>
       <c r="D22" t="str">
         <f>IF(SUMPRODUCT(--(F22:U22&lt;&gt;""))=0,0,"N.A.")</f>
@@ -3222,12 +3248,12 @@
       </c>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>45</v>
       </c>
       <c r="B23" t="str">
-        <f>CONCATENATE("Unit Cost Estimate",IF(C21="Fraction"," (Per 1%)",""))</f>
+        <f>IF(B19="Fixed Cost Program","...",CONCATENATE("Unit Cost Estimate",IF(C21="Fraction"," (Per 1%)","")))</f>
         <v>Unit Cost Estimate (Per 1%)</v>
       </c>
       <c r="C23" t="str">
@@ -3290,12 +3316,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(B19="Latent Cure Program","Efficacy of Vaccination",IF(B19="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B19="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B19="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
+        <f>IF(B19="Fixed Cost Program","...",IF(B19="Latent Cure Program","Efficacy of Cure",IF(B19="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B19="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B19="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","...")))))</f>
         <v>Efficacy of Vaccination</v>
       </c>
       <c r="C24" t="str">
@@ -3311,12 +3337,12 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="str">
-        <f>IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Adherence Probability (Yearly)",IF(B19="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <f>IF(B19="Fixed Cost Program","...",IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Adherence Probability (Yearly)",IF(B19="DS Treatment Program","Adherence Probability (Yearly)","...")))))</f>
         <v>...</v>
       </c>
       <c r="C25" t="str">
@@ -3337,7 +3363,7 @@
         <v>45</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Treatment Duration (Months)",IF(B19="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <f>IF(B19="Fixed Cost Program","...",IF(B19="Latent Cure Program","...",IF(B19="Susceptible Vaccination Program","...",IF(B19="MDR Treatment Program","Treatment Duration (Months)",IF(B19="DS Treatment Program","Treatment Duration (Months)","...")))))</f>
         <v>...</v>
       </c>
       <c r="C26" t="str">
@@ -3359,7 +3385,7 @@
         <v>Latent Cure Program</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.55000000000000004">
@@ -3425,8 +3451,9 @@
       <c r="A30" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
-        <v>47</v>
+      <c r="B30" t="str">
+        <f>IF(B28="Fixed Cost Program","...","Program Coverage")</f>
+        <v>Program Coverage</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
@@ -3450,10 +3477,10 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
         <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
       </c>
       <c r="D31" t="str">
         <f>IF(SUMPRODUCT(--(F31:U31&lt;&gt;""))=0,0,"N.A.")</f>
@@ -3476,7 +3503,7 @@
         <v>45</v>
       </c>
       <c r="B32" t="str">
-        <f>CONCATENATE("Unit Cost Estimate",IF(C30="Fraction"," (Per 1%)",""))</f>
+        <f>IF(B28="Fixed Cost Program","...",CONCATENATE("Unit Cost Estimate",IF(C30="Fraction"," (Per 1%)","")))</f>
         <v>Unit Cost Estimate</v>
       </c>
       <c r="C32" t="str">
@@ -3539,13 +3566,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B33" t="str">
-        <f>IF(B28="Latent Cure Program","Efficacy of Vaccination",IF(B28="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B28="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B28="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","..."))))</f>
-        <v>Efficacy of Vaccination</v>
+        <f>IF(B28="Fixed Cost Program","...",IF(B28="Latent Cure Program","Efficacy of Cure",IF(B28="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B28="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B28="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","...")))))</f>
+        <v>Efficacy of Cure</v>
       </c>
       <c r="C33" t="str">
         <f>IF(B33&lt;&gt;"...","Unique","")</f>
@@ -3560,12 +3587,12 @@
         <v>OR</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>45</v>
       </c>
       <c r="B34" t="str">
-        <f>IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Adherence Probability (Yearly)",IF(B28="DS Treatment Program","Adherence Probability (Yearly)","..."))))</f>
+        <f>IF(B28="Fixed Cost Program","...",IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Adherence Probability (Yearly)",IF(B28="DS Treatment Program","Adherence Probability (Yearly)","...")))))</f>
         <v>...</v>
       </c>
       <c r="C34" t="str">
@@ -3581,12 +3608,12 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>45</v>
       </c>
       <c r="B35" t="str">
-        <f>IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Treatment Duration (Months)",IF(B28="DS Treatment Program","Treatment Duration (Months)","..."))))</f>
+        <f>IF(B28="Fixed Cost Program","...",IF(B28="Latent Cure Program","...",IF(B28="Susceptible Vaccination Program","...",IF(B28="MDR Treatment Program","Treatment Duration (Months)",IF(B28="DS Treatment Program","Treatment Duration (Months)","...")))))</f>
         <v>...</v>
       </c>
       <c r="C35" t="str">
@@ -3602,25 +3629,277 @@
         <v/>
       </c>
     </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="str">
+        <f>'Program Definitions'!$A$6</f>
+        <v>Fixed Cost Program</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38">
+        <v>2000</v>
+      </c>
+      <c r="G38">
+        <v>2001</v>
+      </c>
+      <c r="H38">
+        <v>2002</v>
+      </c>
+      <c r="I38">
+        <v>2003</v>
+      </c>
+      <c r="J38">
+        <v>2004</v>
+      </c>
+      <c r="K38">
+        <v>2005</v>
+      </c>
+      <c r="L38">
+        <v>2006</v>
+      </c>
+      <c r="M38">
+        <v>2007</v>
+      </c>
+      <c r="N38">
+        <v>2008</v>
+      </c>
+      <c r="O38">
+        <v>2009</v>
+      </c>
+      <c r="P38">
+        <v>2010</v>
+      </c>
+      <c r="Q38">
+        <v>2011</v>
+      </c>
+      <c r="R38">
+        <v>2012</v>
+      </c>
+      <c r="S38">
+        <v>2013</v>
+      </c>
+      <c r="T38">
+        <v>2014</v>
+      </c>
+      <c r="U38">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="str">
+        <f>IF(B37="Fixed Cost Program","...","Program Coverage")</f>
+        <v>...</v>
+      </c>
+      <c r="C39" t="str">
+        <f>IF(B39&lt;&gt;"...","Number","")</f>
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <f>IF(B39&lt;&gt;"...",IF(SUMPRODUCT(--(F39:U39&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <f>IF(B39&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40">
+        <f>IF(SUMPRODUCT(--(F40:U40&lt;&gt;""))=0,1000000,"N.A.")</f>
+        <v>1000000</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" t="str">
+        <f>IF(B37="Fixed Cost Program","...",CONCATENATE("Unit Cost Estimate",IF(C39="Fraction"," (Per 1%)","")))</f>
+        <v>...</v>
+      </c>
+      <c r="C41" t="str">
+        <f>IF(B41&lt;&gt;"...","USD","")</f>
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <f>IF(B41&lt;&gt;"...",IF(SUMPRODUCT(--(F41:U41&lt;&gt;"..."))=0,1E+300,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <f>IF(B41&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+      <c r="F41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="G41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="H41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="I41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="J41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="K41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="L41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="N41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="O41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="P41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="Q41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="R41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="S41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="T41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+      <c r="U41" t="str">
+        <f>IF(B41&lt;&gt;"...","...","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="str">
+        <f>IF(B37="Fixed Cost Program","...",IF(B37="Latent Cure Program","Efficacy of Cure",IF(B37="Susceptible Vaccination Program","Efficacy of Vaccination",IF(B37="MDR Treatment Program","Efficacy of treatment (After Treatment Completion)",IF(B37="DS Treatment Program","Efficacy of treatment (After Treatment Completion)","...")))))</f>
+        <v>...</v>
+      </c>
+      <c r="C42" t="str">
+        <f>IF(B42&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <f>IF(B42&lt;&gt;"...",IF(SUMPRODUCT(--(F42:U42&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E42" t="str">
+        <f>IF(B42&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="str">
+        <f>IF(B37="Fixed Cost Program","...",IF(B37="Latent Cure Program","...",IF(B37="Susceptible Vaccination Program","...",IF(B37="MDR Treatment Program","Adherence Probability (Yearly)",IF(B37="DS Treatment Program","Adherence Probability (Yearly)","...")))))</f>
+        <v>...</v>
+      </c>
+      <c r="C43" t="str">
+        <f>IF(B43&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <f>IF(B43&lt;&gt;"...",IF(SUMPRODUCT(--(F43:U43&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E43" t="str">
+        <f>IF(B43&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" t="str">
+        <f>IF(B37="Fixed Cost Program","...",IF(B37="Latent Cure Program","...",IF(B37="Susceptible Vaccination Program","...",IF(B37="MDR Treatment Program","Treatment Duration (Months)",IF(B37="DS Treatment Program","Treatment Duration (Months)","...")))))</f>
+        <v>...</v>
+      </c>
+      <c r="C44" t="str">
+        <f>IF(B44&lt;&gt;"...","Unique","")</f>
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <f>IF(B44&lt;&gt;"...",IF(SUMPRODUCT(--(F44:U44&lt;&gt;""))=0,0,"N.A."),"")</f>
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <f>IF(B44&lt;&gt;"...","OR","")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="9">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C33:C35 C24:C26 C15:C17 C6:C8">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C33:C35 C24:C26 C15:C17 C6:C8 C42:C44">
       <formula1>"Unique"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F32:U32 F23:U23 F14:U14 F5:U5">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F32:U32 F23:U23 F14:U14 F5:U5 F41:U41">
       <formula1>"..."</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C32">
       <formula1>"=CONCATENATE(C31)"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C31 C22 C13 C4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C31 C22 C13 C4 C40:C41">
       <formula1>"USD"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C30 C21 C12 C3">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C30 C21 C12 C3 C39">
       <formula1>"Number,Fraction"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B28 B19 B10 B1">
-      <formula1>"DS Treatment Program,MDR Treatment Program,Susceptible Vaccination Program,Latent Cure Program"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C23">
       <formula1>"=CONCATENATE(C22)"</formula1>
@@ -3630,6 +3909,9 @@
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"=CONCATENATE(C4)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B37 B28 B19 B10 B1">
+      <formula1>"DS Treatment Program,MDR Treatment Program,Susceptible Vaccination Program,Latent Cure Program,Fixed Cost Program"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3709,7 +3991,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3725,7 +4007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3741,7 +4023,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -3757,7 +4039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -3773,7 +4055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3832,7 +4114,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3848,7 +4130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3864,7 +4146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -3880,7 +4162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -3896,7 +4178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -3955,7 +4237,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -3971,7 +4253,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -3987,7 +4269,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4003,7 +4285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4019,7 +4301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -4078,7 +4360,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4094,7 +4376,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4110,7 +4392,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4126,7 +4408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4142,7 +4424,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4403,7 +4685,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4419,7 +4701,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4435,7 +4717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4451,7 +4733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4467,7 +4749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -4526,7 +4808,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4542,7 +4824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4558,7 +4840,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4574,7 +4856,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4590,7 +4872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -4649,7 +4931,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4665,7 +4947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4681,7 +4963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4697,7 +4979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4713,7 +4995,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -4772,7 +5054,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -4797,7 +5079,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -4822,7 +5104,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -4847,7 +5129,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -4872,7 +5154,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -5573,7 +5855,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5589,7 +5871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5617,7 +5899,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5633,7 +5915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5649,7 +5931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -5708,7 +5990,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5724,7 +6006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5743,7 +6025,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5759,7 +6041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5775,7 +6057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5834,7 +6116,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5850,7 +6132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5869,7 +6151,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -5885,7 +6167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -5901,7 +6183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -5960,7 +6242,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="str">
         <f>'Population Definitions'!$A$2</f>
         <v>Children 0-14</v>
@@ -5976,7 +6258,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="str">
         <f>'Population Definitions'!$A$3</f>
         <v>Adults 15-49</v>
@@ -5995,7 +6277,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="str">
         <f>'Population Definitions'!$A$4</f>
         <v>Adults 50+</v>
@@ -6011,7 +6293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="str">
         <f>'Population Definitions'!$A$5</f>
         <v>Prisoners</v>
@@ -6027,7 +6309,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>22</v>
       </c>

</xml_diff>